<commit_message>
[ENH] pabi_pos, supplier consigment report
</commit_message>
<xml_diff>
--- a/pabi_pos/xlsx_template/xlsx_report_supplier_consignment.xlsx
+++ b/pabi_pos/xlsx_template/xlsx_report_supplier_consignment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Supplier Consignment Report</t>
   </si>
@@ -28,10 +28,13 @@
     <t xml:space="preserve">Consigned Supplier</t>
   </si>
   <si>
-    <t xml:space="preserve">From Order Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To Order Date</t>
+    <t xml:space="preserve">From Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Location</t>
   </si>
   <si>
     <t xml:space="preserve">Run Date</t>
@@ -40,6 +43,9 @@
     <t xml:space="preserve">Run By</t>
   </si>
   <si>
+    <t xml:space="preserve">Order Number</t>
+  </si>
+  <si>
     <t xml:space="preserve">Order Date</t>
   </si>
   <si>
@@ -49,19 +55,23 @@
     <t xml:space="preserve">Product Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Sales Location</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount (b/f tax)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -154,41 +164,57 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -208,76 +234,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1006" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="17.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1006" style="4" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6"/>
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>10</v>
+      <c r="F8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>